<commit_message>
increased the amount fo evs a pokemon can have
</commit_message>
<xml_diff>
--- a/Type Effectiveness Chart.xlsx
+++ b/Type Effectiveness Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carmen\Desktop\romhacks\pokemon decomps\Pokemon Indigo League\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F0B412-BA2C-460C-9923-4206AAF46547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E0F339-383D-4924-B3D0-BF9308551741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -617,7 +617,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomRight" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
@@ -1507,7 +1507,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A16" sqref="A16:XFD16"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>

</xml_diff>